<commit_message>
add search in shapes
</commit_message>
<xml_diff>
--- a/text-finder/Result.xlsx
+++ b/text-finder/Result.xlsx
@@ -14,19 +14,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>tokyo</t>
+    <t>shape 1</t>
   </si>
   <si>
-    <t>B6</t>
+    <t/>
   </si>
   <si>
     <t>Sheet1</t>
   </si>
   <si>
-    <t>search.xlsx</t>
+    <t>2021091611DocumentBeek1.xlsx</t>
   </si>
   <si>
-    <t>C:\excel-files\search.xlsx</t>
+    <t>C:\excel-files\2021091611DocumentBeek1.xlsx</t>
   </si>
 </sst>
 </file>

</xml_diff>